<commit_message>
An attempt at graph-based contact tracing.
</commit_message>
<xml_diff>
--- a/VIC_2/input/calculations/Starting popn by vaccine status.xlsx
+++ b/VIC_2/input/calculations/Starting popn by vaccine status.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud.sharepoint.com/teams/COVID-19Planningpathtosuppresselim/Shared Documents/General/1PI/Publications/1112_ABM-PMSLT Vic Vaccine Borders Obj 3b/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\VIC_2\input\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E1C00A23-A827-45E1-B318-02523865D6F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8249633-30CA-40FB-AE51-33F4050476E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="population" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -218,7 +229,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -780,7 +791,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Tony Blakely" refreshedDate="44348.512562037038" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="35">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Tony Blakely" refreshedDate="44348.512562037038" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="35" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:R36" sheet="population"/>
   </cacheSource>
@@ -1565,7 +1576,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField dataField="1" showAll="0"/>
@@ -1962,22 +1973,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>62</v>
       </c>
@@ -1989,7 +2001,7 @@
       </c>
       <c r="P2" s="9"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -2026,7 +2038,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>15</v>
       </c>
@@ -2134,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>25</v>
       </c>
@@ -2189,7 +2201,7 @@
       </c>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>35</v>
       </c>
@@ -2244,7 +2256,7 @@
       </c>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45</v>
       </c>
@@ -2299,7 +2311,7 @@
       </c>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>55</v>
       </c>
@@ -2354,7 +2366,7 @@
       </c>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>65</v>
       </c>
@@ -2409,7 +2421,7 @@
       </c>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>75</v>
       </c>
@@ -2464,7 +2476,7 @@
       </c>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>85</v>
       </c>
@@ -2519,7 +2531,7 @@
       </c>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>95</v>
       </c>
@@ -2574,7 +2586,7 @@
       </c>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -2602,7 +2614,7 @@
         <v>355.75</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
         <v>53</v>
       </c>
@@ -2611,12 +2623,12 @@
         <v>350.33962264150944</v>
       </c>
     </row>
-    <row r="18" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>56</v>
       </c>
@@ -2624,7 +2636,7 @@
         <v>26500000</v>
       </c>
     </row>
-    <row r="20" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>54</v>
       </c>
@@ -2640,7 +2652,7 @@
         <v>0.49486285229522103</v>
       </c>
     </row>
-    <row r="21" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>55</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>2.6666666666666668E-2</v>
       </c>
     </row>
-    <row r="22" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>57</v>
       </c>
@@ -2673,12 +2685,12 @@
         <v>0.16018113207547172</v>
       </c>
     </row>
-    <row r="23" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="10:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:18" x14ac:dyDescent="0.25">
       <c r="N25">
         <f>SUM(N21:N22)/N19</f>
         <v>0.14013584905660378</v>
@@ -2691,16 +2703,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2756,7 +2768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2812,7 +2824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2868,7 +2880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2924,7 +2936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>22</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -3036,7 +3048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>17</v>
       </c>
@@ -3092,7 +3104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>36</v>
       </c>
@@ -3148,7 +3160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3204,7 +3216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>27</v>
       </c>
@@ -3260,7 +3272,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3316,7 +3328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -3372,7 +3384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -3428,7 +3440,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16</v>
       </c>
@@ -3484,7 +3496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3540,7 +3552,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -3596,7 +3608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>180</v>
       </c>
@@ -3652,7 +3664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>82</v>
       </c>
@@ -3708,7 +3720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -3764,7 +3776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3820,7 +3832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3876,7 +3888,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>44</v>
       </c>
@@ -3932,7 +3944,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>44</v>
       </c>
@@ -3988,7 +4000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>39</v>
       </c>
@@ -4044,7 +4056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>37</v>
       </c>
@@ -4100,7 +4112,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>31</v>
       </c>
@@ -4156,7 +4168,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -4212,7 +4224,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -4324,7 +4336,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>301</v>
       </c>
@@ -4380,7 +4392,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>256</v>
       </c>
@@ -4436,7 +4448,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>240</v>
       </c>
@@ -4492,7 +4504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>215</v>
       </c>
@@ -4548,7 +4560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>191</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>330</v>
       </c>
@@ -4660,7 +4672,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>222</v>
       </c>

</xml_diff>

<commit_message>
Added recursive tracking. Set vaccine proportion and rollout rate to match the specifications.
</commit_message>
<xml_diff>
--- a/VIC_2/input/calculations/Starting popn by vaccine status.xlsx
+++ b/VIC_2/input/calculations/Starting popn by vaccine status.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\VIC_2\input\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8249633-30CA-40FB-AE51-33F4050476E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863D64A6-3679-45D4-A239-22E2165A7003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="population" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="population" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
   <si>
     <t>totalAgents</t>
   </si>
@@ -224,6 +225,21 @@
   </si>
   <si>
     <t>Vaccination coverage (one or two doses)</t>
+  </si>
+  <si>
+    <t>Dose 1</t>
+  </si>
+  <si>
+    <t>Dose 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population </t>
+  </si>
+  <si>
+    <t>Vac Cover</t>
+  </si>
+  <si>
+    <t>Vac Essential</t>
   </si>
 </sst>
 </file>
@@ -718,7 +734,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -731,6 +747,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1973,11 +1992,2080 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7C0653-18B5-40D5-BABB-4FD63F2D1C5D}">
+  <dimension ref="A3:N62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="9.5703125" style="3" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="3">
+        <v>6681000</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1063120</v>
+      </c>
+      <c r="C4" s="10">
+        <f>B4/B3</f>
+        <v>0.15912587935937733</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="10">
+        <v>111928</v>
+      </c>
+      <c r="C5" s="10">
+        <f>B5/B3</f>
+        <v>1.6753180661577608E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>330</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>B11-C11</f>
+        <v>330</v>
+      </c>
+      <c r="E11">
+        <f>C11</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <f>ROUND(F11*D11, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <f>ROUND(G11*E11, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>222</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>B12-C12</f>
+        <v>222</v>
+      </c>
+      <c r="E12">
+        <f>C12</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <f>ROUND(F12*D12, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <f>ROUND(G12*E12, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>384</v>
+      </c>
+      <c r="C13">
+        <v>85</v>
+      </c>
+      <c r="D13">
+        <f>B13-C13</f>
+        <v>299</v>
+      </c>
+      <c r="E13">
+        <f>C13</f>
+        <v>85</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="H13" s="3">
+        <f>ROUND(F13*D13, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <f>ROUND(G13*E13, 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>345</v>
+      </c>
+      <c r="C14">
+        <v>73</v>
+      </c>
+      <c r="D14">
+        <f>B14-C14</f>
+        <v>272</v>
+      </c>
+      <c r="E14">
+        <f>C14</f>
+        <v>73</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="H14" s="3">
+        <f>ROUND(F14*D14, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <f>ROUND(G14*E14, 0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>304</v>
+      </c>
+      <c r="C15">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <f>B15-C15</f>
+        <v>240</v>
+      </c>
+      <c r="E15">
+        <f>C15</f>
+        <v>64</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="H15" s="3">
+        <f>ROUND(F15*D15, 0)</f>
+        <v>12</v>
+      </c>
+      <c r="I15" s="3">
+        <f>ROUND(G15*E15, 0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>342</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>B16-C16</f>
+        <v>342</v>
+      </c>
+      <c r="E16">
+        <f>C16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <f>ROUND(F16*D16, 0)</f>
+        <v>68</v>
+      </c>
+      <c r="I16" s="3">
+        <f>ROUND(G16*E16, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>291</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>B17-C17</f>
+        <v>291</v>
+      </c>
+      <c r="E17">
+        <f>C17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <f>ROUND(F17*D17, 0)</f>
+        <v>73</v>
+      </c>
+      <c r="I17" s="3">
+        <f>ROUND(G17*E17, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <v>180</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>B18-C18</f>
+        <v>180</v>
+      </c>
+      <c r="E18">
+        <f>C18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <f>ROUND(F18*D18, 0)</f>
+        <v>99</v>
+      </c>
+      <c r="I18" s="3">
+        <f>ROUND(G18*E18, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>82</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>B19-C19</f>
+        <v>82</v>
+      </c>
+      <c r="E19">
+        <f>C19</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <f>ROUND(F19*D19, 0)</f>
+        <v>49</v>
+      </c>
+      <c r="I19" s="3">
+        <f>ROUND(G19*E19, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>95</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>B20-C20</f>
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <f>C20</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <f>ROUND(F20*D20, 0)</f>
+        <v>14</v>
+      </c>
+      <c r="I20" s="3">
+        <f>ROUND(G20*E20, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <f>SUM(B11:B20)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H23" s="3">
+        <f>SUM(H11:I20)</f>
+        <v>376</v>
+      </c>
+      <c r="I23" s="3">
+        <f>SUM(N28:N62)</f>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H24" s="3">
+        <f>H23/B22</f>
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="I24" s="3">
+        <f>I23/B22</f>
+        <v>0.15040000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f>ROUND(G13*E28,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f>ROUND(G14*E29,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>45</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f>ROUND(G15*E30,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>22</v>
+      </c>
+      <c r="F31">
+        <v>22</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <f>ROUND(G13*E31,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>35</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f>ROUND(G14*E32,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>17</v>
+      </c>
+      <c r="F33">
+        <v>17</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f>ROUND(G15*E33,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>36</v>
+      </c>
+      <c r="F34">
+        <v>36</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f>ROUND(G13*E34,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>30</v>
+      </c>
+      <c r="F35">
+        <v>30</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f>ROUND(G14*E35,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>27</v>
+      </c>
+      <c r="F36">
+        <v>27</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f>ROUND(G15*E36,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <f>ROUND(G13*E37,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <f>ROUND(G14*E38,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <f>ROUND(G15*E39,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>16</v>
+      </c>
+      <c r="F40">
+        <v>16</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <f>ROUND(G13*E40,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>35</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <v>15</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <f>ROUND(G14*E41,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>13</v>
+      </c>
+      <c r="F42">
+        <v>13</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+      <c r="N42">
+        <f>ROUND(G15*E42,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>180</v>
+      </c>
+      <c r="B43">
+        <v>75</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>23</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>2</v>
+      </c>
+      <c r="N43">
+        <f>ROUND(F18*A43,0)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <v>85</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>12</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <f>ROUND(F19*A44,0)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>95</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <f>ROUND(F20*A45,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>55</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <f>ROUND(F16*A46,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>65</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <f>ROUND(F17*A47,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>35</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <f>ROUND(F13*A48,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49">
+        <v>35</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>35</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <f>ROUND(F14*A49,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50">
+        <v>45</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>31</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <f>ROUND(F15*A50,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>37</v>
+      </c>
+      <c r="B51">
+        <v>55</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>23</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <f>ROUND(F16*A51,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>31</v>
+      </c>
+      <c r="B52">
+        <v>65</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <f>ROUND(F17*A52,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>25</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>12</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <f>ROUND(F13*A53,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>13</v>
+      </c>
+      <c r="B54">
+        <v>35</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>10</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <f>ROUND(F14*A54,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>45</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <f>ROUND(F15*A55,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>301</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>187</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <f>ROUND(F16*A56,0)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>256</v>
+      </c>
+      <c r="B57">
+        <v>65</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>60</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <f>ROUND(F17*A57,0)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>240</v>
+      </c>
+      <c r="B58">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>190</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <f>ROUND(F13*A58,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>215</v>
+      </c>
+      <c r="B59">
+        <v>35</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>173</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <f>ROUND(F14*A59,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>191</v>
+      </c>
+      <c r="B60">
+        <v>45</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>154</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <f>ROUND(F15*A60,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>330</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M61">
+        <v>2</v>
+      </c>
+      <c r="N61">
+        <f>ROUND(F11*A61,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>222</v>
+      </c>
+      <c r="B62">
+        <v>15</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <f>ROUND(F12*A62,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,6 +4073,10 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -2702,7 +4794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>

</xml_diff>